<commit_message>
created Worksheets based on subcontrollers
</commit_message>
<xml_diff>
--- a/TaglistCreatorFromIGS/bin/Debug/Resources/StandardTagList.xlsx
+++ b/TaglistCreatorFromIGS/bin/Debug/Resources/StandardTagList.xlsx
@@ -5,14 +5,14 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212478881\Documents\Visual Studio 2015\Projects\TestConsoleApplication\TestConsoleApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212478881\Documents\Visual Studio 2015\Projects\TaglistCreatorFromIGS\TaglistCreatorFromIGS\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="926"/>
   </bookViews>
   <sheets>
-    <sheet name="ZW1" sheetId="3" r:id="rId1"/>
+    <sheet name="Template" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -51,10 +51,10 @@
     <t>On-site Value</t>
   </si>
   <si>
-    <t>ZW1</t>
+    <t>Comments</t>
   </si>
   <si>
-    <t>Comments</t>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -10097,11 +10097,12 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -10156,7 +10157,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -10170,7 +10171,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>